<commit_message>
All bar_graphs showing correctly
</commit_message>
<xml_diff>
--- a/word_categories.xlsx
+++ b/word_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hokuatarnas/Documents/LING270/final_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43CB672-0BF7-9741-9ED2-AEABE1632611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4703C9F6-6B67-0347-87C3-F91883CE77B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16760" xr2:uid="{773B45D8-DFA8-2742-BE2D-A032334DE3ED}"/>
+    <workbookView xWindow="13400" yWindow="460" windowWidth="15020" windowHeight="16760" xr2:uid="{773B45D8-DFA8-2742-BE2D-A032334DE3ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,26 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="143">
   <si>
     <t>Word</t>
   </si>
   <si>
-    <t>* C = consonant *</t>
-  </si>
-  <si>
-    <t>* all "i" *</t>
-  </si>
-  <si>
     <t>sCC</t>
   </si>
   <si>
     <t>i</t>
   </si>
   <si>
-    <t>ŋ / ŋk (nasal)</t>
-  </si>
-  <si>
     <t>skring</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>strunk</t>
   </si>
   <si>
-    <t>k / g</t>
-  </si>
-  <si>
     <t>strick</t>
   </si>
   <si>
@@ -105,15 +93,9 @@
     <t>strug</t>
   </si>
   <si>
-    <t>n / m</t>
-  </si>
-  <si>
     <t>skrim</t>
   </si>
   <si>
-    <t>skrimed</t>
-  </si>
-  <si>
     <t>skram</t>
   </si>
   <si>
@@ -132,15 +114,9 @@
     <t>sprun</t>
   </si>
   <si>
-    <t>C (other consonant)</t>
-  </si>
-  <si>
     <t>spriv</t>
   </si>
   <si>
-    <t>sprived</t>
-  </si>
-  <si>
     <t>sprav</t>
   </si>
   <si>
@@ -456,24 +432,12 @@
     <t>kub</t>
   </si>
   <si>
-    <t>*Category C*</t>
-  </si>
-  <si>
-    <t>*Category B*</t>
-  </si>
-  <si>
-    <t>*Category A*</t>
-  </si>
-  <si>
     <t>A. "-ed"</t>
   </si>
   <si>
     <t>B. "/æ/"</t>
   </si>
   <si>
-    <t xml:space="preserve">C. "/ʌ/" </t>
-  </si>
-  <si>
     <t>middle_vowels</t>
   </si>
   <si>
@@ -481,13 +445,31 @@
   </si>
   <si>
     <t>initial_consonants</t>
+  </si>
+  <si>
+    <t>C. "/ʌ/"</t>
+  </si>
+  <si>
+    <t>skrimmed</t>
+  </si>
+  <si>
+    <t>sprivved</t>
+  </si>
+  <si>
+    <t>nasal</t>
+  </si>
+  <si>
+    <t>k/g</t>
+  </si>
+  <si>
+    <t>n/m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,13 +479,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -542,12 +517,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3AC5CF-40E3-4C47-B0FB-0A2D0B953869}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,25 +854,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -908,764 +882,737 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="G19" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="A21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>4</v>
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>4</v>
+      <c r="A25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="A28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="A29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="A30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="A31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>4</v>
+      <c r="A32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>4</v>
+      <c r="A33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>